<commit_message>
conditional formatting remains for step 2
</commit_message>
<xml_diff>
--- a/bot_outputs/step_1_out.xlsx
+++ b/bot_outputs/step_1_out.xlsx
@@ -11385,23 +11385,24 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="4" t="inlineStr">
         <is>
           <t>Database Name</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="4" t="inlineStr">
         <is>
           <t>LOS Name</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="4" t="inlineStr">
         <is>
           <t>PHDWIN Id</t>
         </is>

</xml_diff>